<commit_message>
Add point 2.3 - accumulating and "averaging"
</commit_message>
<xml_diff>
--- a/Cv04/LedInBinary.xlsx
+++ b/Cv04/LedInBinary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NovotnyJ\Documents\MKSCviceni\Cv04\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6B563087-32AE-426D-8772-866302B462AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23C5F23F-A006-4556-837A-1610E5BB826D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{4D4C8CE9-6CB2-4554-BEE3-24423AD56172}"/>
   </bookViews>
@@ -391,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8194E61A-B66A-4A85-A5A3-9A081938A298}">
-  <dimension ref="F12:AA21"/>
+  <dimension ref="F12:AA50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AC19" sqref="AC19"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="W57" sqref="W57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1149,6 +1149,597 @@
         <v>11111111</v>
       </c>
     </row>
+    <row r="30" spans="6:27" x14ac:dyDescent="0.35">
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>10</v>
+      </c>
+      <c r="I30">
+        <v>20</v>
+      </c>
+      <c r="J30">
+        <v>30</v>
+      </c>
+      <c r="K30">
+        <v>40</v>
+      </c>
+      <c r="L30">
+        <v>50</v>
+      </c>
+      <c r="M30">
+        <v>60</v>
+      </c>
+      <c r="N30">
+        <v>70</v>
+      </c>
+      <c r="O30">
+        <v>80</v>
+      </c>
+      <c r="P30">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="31" spans="6:27" x14ac:dyDescent="0.35">
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <f>$F31+G$30</f>
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <f t="shared" ref="H31:P36" si="13">$F31+H$30</f>
+        <v>10</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="13"/>
+        <v>20</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="13"/>
+        <v>30</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="13"/>
+        <v>40</v>
+      </c>
+      <c r="L31">
+        <f t="shared" si="13"/>
+        <v>50</v>
+      </c>
+      <c r="M31">
+        <f t="shared" si="13"/>
+        <v>60</v>
+      </c>
+      <c r="N31">
+        <f t="shared" si="13"/>
+        <v>70</v>
+      </c>
+      <c r="O31">
+        <f t="shared" si="13"/>
+        <v>80</v>
+      </c>
+      <c r="P31">
+        <f t="shared" si="13"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="32" spans="6:27" x14ac:dyDescent="0.35">
+      <c r="F32">
+        <v>100</v>
+      </c>
+      <c r="G32">
+        <f t="shared" ref="G32:G36" si="14">$F32+G$30</f>
+        <v>100</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="13"/>
+        <v>110</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="13"/>
+        <v>120</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="13"/>
+        <v>130</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="13"/>
+        <v>140</v>
+      </c>
+      <c r="L32">
+        <f t="shared" si="13"/>
+        <v>150</v>
+      </c>
+      <c r="M32">
+        <f t="shared" si="13"/>
+        <v>160</v>
+      </c>
+      <c r="N32">
+        <f t="shared" si="13"/>
+        <v>170</v>
+      </c>
+      <c r="O32">
+        <f t="shared" si="13"/>
+        <v>180</v>
+      </c>
+      <c r="P32">
+        <f t="shared" si="13"/>
+        <v>190</v>
+      </c>
+    </row>
+    <row r="33" spans="6:22" x14ac:dyDescent="0.35">
+      <c r="F33">
+        <v>200</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="14"/>
+        <v>200</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="13"/>
+        <v>210</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="13"/>
+        <v>220</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="13"/>
+        <v>230</v>
+      </c>
+      <c r="K33">
+        <f t="shared" si="13"/>
+        <v>240</v>
+      </c>
+      <c r="L33">
+        <f t="shared" si="13"/>
+        <v>250</v>
+      </c>
+      <c r="M33">
+        <f t="shared" si="13"/>
+        <v>260</v>
+      </c>
+      <c r="N33">
+        <f t="shared" si="13"/>
+        <v>270</v>
+      </c>
+      <c r="O33">
+        <f t="shared" si="13"/>
+        <v>280</v>
+      </c>
+      <c r="P33">
+        <f t="shared" si="13"/>
+        <v>290</v>
+      </c>
+    </row>
+    <row r="34" spans="6:22" x14ac:dyDescent="0.35">
+      <c r="F34">
+        <v>300</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="14"/>
+        <v>300</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="13"/>
+        <v>310</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="13"/>
+        <v>320</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="13"/>
+        <v>330</v>
+      </c>
+      <c r="K34">
+        <f t="shared" si="13"/>
+        <v>340</v>
+      </c>
+      <c r="L34">
+        <f t="shared" si="13"/>
+        <v>350</v>
+      </c>
+      <c r="M34">
+        <f t="shared" si="13"/>
+        <v>360</v>
+      </c>
+      <c r="N34">
+        <f t="shared" si="13"/>
+        <v>370</v>
+      </c>
+      <c r="O34">
+        <f t="shared" si="13"/>
+        <v>380</v>
+      </c>
+      <c r="P34">
+        <f t="shared" si="13"/>
+        <v>390</v>
+      </c>
+    </row>
+    <row r="35" spans="6:22" x14ac:dyDescent="0.35">
+      <c r="F35">
+        <v>400</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="14"/>
+        <v>400</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="13"/>
+        <v>410</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="13"/>
+        <v>420</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="13"/>
+        <v>430</v>
+      </c>
+      <c r="K35">
+        <f t="shared" si="13"/>
+        <v>440</v>
+      </c>
+      <c r="L35">
+        <f t="shared" si="13"/>
+        <v>450</v>
+      </c>
+      <c r="M35">
+        <f t="shared" si="13"/>
+        <v>460</v>
+      </c>
+      <c r="N35">
+        <f t="shared" si="13"/>
+        <v>470</v>
+      </c>
+      <c r="O35">
+        <f t="shared" si="13"/>
+        <v>480</v>
+      </c>
+      <c r="P35">
+        <f t="shared" si="13"/>
+        <v>490</v>
+      </c>
+    </row>
+    <row r="36" spans="6:22" x14ac:dyDescent="0.35">
+      <c r="F36">
+        <v>500</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="14"/>
+        <v>500</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="13"/>
+        <v>510</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="13"/>
+        <v>520</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="13"/>
+        <v>530</v>
+      </c>
+      <c r="K36">
+        <f t="shared" si="13"/>
+        <v>540</v>
+      </c>
+      <c r="L36">
+        <f t="shared" si="13"/>
+        <v>550</v>
+      </c>
+      <c r="M36">
+        <f t="shared" si="13"/>
+        <v>560</v>
+      </c>
+      <c r="N36">
+        <f t="shared" si="13"/>
+        <v>570</v>
+      </c>
+      <c r="O36">
+        <f t="shared" si="13"/>
+        <v>580</v>
+      </c>
+      <c r="P36">
+        <f t="shared" si="13"/>
+        <v>590</v>
+      </c>
+    </row>
+    <row r="40" spans="6:22" x14ac:dyDescent="0.35">
+      <c r="G40">
+        <f>QUOTIENT(G31,QUOTIENT(500,9))</f>
+        <v>0</v>
+      </c>
+      <c r="H40">
+        <f t="shared" ref="H40:P40" si="15">QUOTIENT(H31,QUOTIENT(500,9))</f>
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="J40">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="K40">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="L40">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="M40">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+      <c r="N40">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+      <c r="O40">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+      <c r="P40">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="6:22" x14ac:dyDescent="0.35">
+      <c r="G41">
+        <f t="shared" ref="G41:P41" si="16">QUOTIENT(G32,QUOTIENT(500,9))</f>
+        <v>1</v>
+      </c>
+      <c r="H41">
+        <f t="shared" si="16"/>
+        <v>2</v>
+      </c>
+      <c r="I41">
+        <f t="shared" si="16"/>
+        <v>2</v>
+      </c>
+      <c r="J41">
+        <f t="shared" si="16"/>
+        <v>2</v>
+      </c>
+      <c r="K41">
+        <f t="shared" si="16"/>
+        <v>2</v>
+      </c>
+      <c r="L41">
+        <f t="shared" si="16"/>
+        <v>2</v>
+      </c>
+      <c r="M41">
+        <f t="shared" si="16"/>
+        <v>2</v>
+      </c>
+      <c r="N41">
+        <f t="shared" si="16"/>
+        <v>3</v>
+      </c>
+      <c r="O41">
+        <f t="shared" si="16"/>
+        <v>3</v>
+      </c>
+      <c r="P41">
+        <f t="shared" si="16"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="6:22" x14ac:dyDescent="0.35">
+      <c r="G42">
+        <f t="shared" ref="G42:P42" si="17">QUOTIENT(G33,QUOTIENT(500,9))</f>
+        <v>3</v>
+      </c>
+      <c r="H42">
+        <f t="shared" si="17"/>
+        <v>3</v>
+      </c>
+      <c r="I42">
+        <f t="shared" si="17"/>
+        <v>4</v>
+      </c>
+      <c r="J42">
+        <f t="shared" si="17"/>
+        <v>4</v>
+      </c>
+      <c r="K42">
+        <f t="shared" si="17"/>
+        <v>4</v>
+      </c>
+      <c r="L42">
+        <f t="shared" si="17"/>
+        <v>4</v>
+      </c>
+      <c r="M42">
+        <f t="shared" si="17"/>
+        <v>4</v>
+      </c>
+      <c r="N42">
+        <f t="shared" si="17"/>
+        <v>4</v>
+      </c>
+      <c r="O42">
+        <f t="shared" si="17"/>
+        <v>5</v>
+      </c>
+      <c r="P42">
+        <f t="shared" si="17"/>
+        <v>5</v>
+      </c>
+      <c r="U42">
+        <v>0</v>
+      </c>
+      <c r="V42">
+        <f>COUNTIF($G$40:$P$45,U42)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="6:22" x14ac:dyDescent="0.35">
+      <c r="G43">
+        <f t="shared" ref="G43:P43" si="18">QUOTIENT(G34,QUOTIENT(500,9))</f>
+        <v>5</v>
+      </c>
+      <c r="H43">
+        <f t="shared" si="18"/>
+        <v>5</v>
+      </c>
+      <c r="I43">
+        <f t="shared" si="18"/>
+        <v>5</v>
+      </c>
+      <c r="J43">
+        <f t="shared" si="18"/>
+        <v>6</v>
+      </c>
+      <c r="K43">
+        <f t="shared" si="18"/>
+        <v>6</v>
+      </c>
+      <c r="L43">
+        <f t="shared" si="18"/>
+        <v>6</v>
+      </c>
+      <c r="M43">
+        <f t="shared" si="18"/>
+        <v>6</v>
+      </c>
+      <c r="N43">
+        <f t="shared" si="18"/>
+        <v>6</v>
+      </c>
+      <c r="O43">
+        <f t="shared" si="18"/>
+        <v>6</v>
+      </c>
+      <c r="P43">
+        <f t="shared" si="18"/>
+        <v>7</v>
+      </c>
+      <c r="U43">
+        <v>1</v>
+      </c>
+      <c r="V43">
+        <f t="shared" ref="V43:V50" si="19">COUNTIF($G$40:$P$45,U43)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="6:22" x14ac:dyDescent="0.35">
+      <c r="G44">
+        <f t="shared" ref="G44:P44" si="20">QUOTIENT(G35,QUOTIENT(500,9))</f>
+        <v>7</v>
+      </c>
+      <c r="H44">
+        <f t="shared" si="20"/>
+        <v>7</v>
+      </c>
+      <c r="I44">
+        <f t="shared" si="20"/>
+        <v>7</v>
+      </c>
+      <c r="J44">
+        <f t="shared" si="20"/>
+        <v>7</v>
+      </c>
+      <c r="K44">
+        <f t="shared" si="20"/>
+        <v>8</v>
+      </c>
+      <c r="L44">
+        <f t="shared" si="20"/>
+        <v>8</v>
+      </c>
+      <c r="M44">
+        <f t="shared" si="20"/>
+        <v>8</v>
+      </c>
+      <c r="N44">
+        <f t="shared" si="20"/>
+        <v>8</v>
+      </c>
+      <c r="O44">
+        <f t="shared" si="20"/>
+        <v>8</v>
+      </c>
+      <c r="P44">
+        <f t="shared" si="20"/>
+        <v>8</v>
+      </c>
+      <c r="U44">
+        <v>2</v>
+      </c>
+      <c r="V44">
+        <f t="shared" si="19"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="6:22" x14ac:dyDescent="0.35">
+      <c r="G45">
+        <f t="shared" ref="G45:P45" si="21">QUOTIENT(G36,QUOTIENT(500,9))</f>
+        <v>9</v>
+      </c>
+      <c r="U45">
+        <v>3</v>
+      </c>
+      <c r="V45">
+        <f t="shared" si="19"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="6:22" x14ac:dyDescent="0.35">
+      <c r="U46">
+        <v>4</v>
+      </c>
+      <c r="V46">
+        <f t="shared" si="19"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="6:22" x14ac:dyDescent="0.35">
+      <c r="U47">
+        <v>5</v>
+      </c>
+      <c r="V47">
+        <f t="shared" si="19"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="6:22" x14ac:dyDescent="0.35">
+      <c r="U48">
+        <v>6</v>
+      </c>
+      <c r="V48">
+        <f t="shared" si="19"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="21:22" x14ac:dyDescent="0.35">
+      <c r="U49">
+        <v>7</v>
+      </c>
+      <c r="V49">
+        <f t="shared" si="19"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="21:22" x14ac:dyDescent="0.35">
+      <c r="U50">
+        <v>8</v>
+      </c>
+      <c r="V50">
+        <f t="shared" si="19"/>
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>